<commit_message>
adding another fied in excel
</commit_message>
<xml_diff>
--- a/templates/client_dashboard.xlsx
+++ b/templates/client_dashboard.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harika\Documents\Tattva cap\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09701B8A-AE18-474D-B48B-58550C232671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1064D9F1-AB31-47FB-87E1-87DBD6E277F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1848" yWindow="1848" windowWidth="17280" windowHeight="8880" xr2:uid="{955A2D66-0C82-4C00-8837-76C14ED94AA4}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{955A2D66-0C82-4C00-8837-76C14ED94AA4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>client_code</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>Harika</t>
+  </si>
+  <si>
+    <t>others</t>
   </si>
 </sst>
 </file>
@@ -419,10 +422,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D1890A-EAB5-41AE-909B-E1F723185C83}">
-  <dimension ref="A1:I2"/>
+  <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K9" sqref="K9"/>
+      <selection activeCell="O4" sqref="O4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -438,7 +441,7 @@
     <col min="9" max="9" width="7.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,8 +469,11 @@
       <c r="I1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" t="s">
+        <v>10</v>
+      </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>83030088</v>
       </c>
@@ -494,6 +500,9 @@
       </c>
       <c r="I2">
         <v>5</v>
+      </c>
+      <c r="J2">
+        <v>2000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
adding another fied in excel 1
</commit_message>
<xml_diff>
--- a/templates/client_dashboard.xlsx
+++ b/templates/client_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harika\Documents\Tattva cap\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1064D9F1-AB31-47FB-87E1-87DBD6E277F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF28B2-4E19-4910-BAAB-5441B581A1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{955A2D66-0C82-4C00-8837-76C14ED94AA4}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O4" sqref="O4"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -481,25 +481,25 @@
         <v>9</v>
       </c>
       <c r="C2" s="1">
-        <v>45817</v>
+        <v>45818</v>
       </c>
       <c r="D2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="E2">
+        <v>11000</v>
+      </c>
+      <c r="F2">
+        <v>5</v>
+      </c>
+      <c r="G2">
         <v>5000</v>
       </c>
-      <c r="F2">
-        <v>2</v>
-      </c>
-      <c r="G2">
-        <v>200</v>
-      </c>
       <c r="H2">
-        <v>2000</v>
+        <v>22000</v>
       </c>
       <c r="I2">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="J2">
         <v>2000</v>
@@ -507,5 +507,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
adding another fied in excel 2
</commit_message>
<xml_diff>
--- a/templates/client_dashboard.xlsx
+++ b/templates/client_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harika\Documents\Tattva cap\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EDF28B2-4E19-4910-BAAB-5441B581A1EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87201C74-8704-40CF-AE9B-7F02C67A00F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{955A2D66-0C82-4C00-8837-76C14ED94AA4}"/>
   </bookViews>
@@ -425,7 +425,7 @@
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
adding another fied in excel 8
</commit_message>
<xml_diff>
--- a/templates/client_dashboard.xlsx
+++ b/templates/client_dashboard.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Harika\Documents\Tattva cap\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87201C74-8704-40CF-AE9B-7F02C67A00F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D5A91C5-74B5-4616-AA8A-92BC30516276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{955A2D66-0C82-4C00-8837-76C14ED94AA4}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>client_code</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>others</t>
+  </si>
+  <si>
+    <t>Kalpana</t>
   </si>
 </sst>
 </file>
@@ -422,10 +425,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E6D1890A-EAB5-41AE-909B-E1F723185C83}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,6 +508,38 @@
         <v>2000</v>
       </c>
     </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>83030000</v>
+      </c>
+      <c r="B3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="1">
+        <v>45819</v>
+      </c>
+      <c r="D3">
+        <v>1000</v>
+      </c>
+      <c r="E3">
+        <v>11000</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>6000</v>
+      </c>
+      <c r="H3">
+        <v>2000</v>
+      </c>
+      <c r="I3">
+        <v>8</v>
+      </c>
+      <c r="J3">
+        <v>5000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>